<commit_message>
Shiny main page BETA1.0
</commit_message>
<xml_diff>
--- a/datasett/Norway/norway_format.xlsx
+++ b/datasett/Norway/norway_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumenter\Google Drive\NHH\Master\BAN400\TermPaper\datasett\Norway\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit-my.sharepoint.com/personal/olai_viken_student_nhh_no/Documents/MASTER/BAN400/Term paper/BAN400-term-paper/datasett/Norway/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14CF15E-E628-4411-933B-CCA3F4E5AA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D14CF15E-E628-4411-933B-CCA3F4E5AA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E765C438-52E0-BB4A-9A7C-9FA33269E56B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Gender</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Gender Column</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -361,15 +367,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,17 +383,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -401,9 +410,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>

</xml_diff>